<commit_message>
DAS - R-1 - Sensitivity analysis excel
</commit_message>
<xml_diff>
--- a/Reviewer_Comments_R_1_24-Dec-2024.xlsx
+++ b/Reviewer_Comments_R_1_24-Dec-2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PhD\Publications\Research_Article_REINFORCE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71B846A0-F55C-4354-B780-6BE62A12349D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BEBAB74-0291-40E9-8B90-70ACBDA75C80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="414" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="414" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="6" r:id="rId1"/>
@@ -3622,46 +3622,46 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4898,12 +4898,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{816F3457-95CC-4A5E-96D0-1EA42C9E78DF}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:O24"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E25" sqref="E25"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4960,7 +4959,7 @@
       </c>
       <c r="O1" s="86"/>
     </row>
-    <row r="2" spans="1:15" ht="16.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="73" t="s">
         <v>105</v>
       </c>
@@ -4999,7 +4998,7 @@
       </c>
       <c r="O2" s="87"/>
     </row>
-    <row r="3" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="16.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="74" t="s">
         <v>23</v>
       </c>
@@ -5042,7 +5041,7 @@
       </c>
       <c r="O3" s="87"/>
     </row>
-    <row r="4" spans="1:15" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="74" t="s">
         <v>23</v>
       </c>
@@ -5162,7 +5161,7 @@
       </c>
       <c r="O6" s="87"/>
     </row>
-    <row r="7" spans="1:15" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="74" t="s">
         <v>23</v>
       </c>
@@ -5225,7 +5224,7 @@
       </c>
       <c r="K8" s="164">
         <f ca="1">TODAY()</f>
-        <v>45650</v>
+        <v>45652</v>
       </c>
       <c r="L8" s="164"/>
       <c r="M8" s="87"/>
@@ -5257,14 +5256,14 @@
       </c>
       <c r="K9" s="87">
         <f ca="1">K7-K8-1</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="L9" s="102"/>
       <c r="M9" s="87"/>
       <c r="N9" s="87"/>
       <c r="O9" s="87"/>
     </row>
-    <row r="10" spans="1:15" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="74" t="s">
         <v>23</v>
       </c>
@@ -5384,7 +5383,7 @@
       <c r="N13" s="143"/>
       <c r="O13" s="87"/>
     </row>
-    <row r="14" spans="1:15" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="74"/>
       <c r="B14" s="66">
         <v>2</v>
@@ -5440,7 +5439,7 @@
       <c r="N15" s="148"/>
       <c r="O15" s="87"/>
     </row>
-    <row r="16" spans="1:15" ht="16.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="74" t="s">
         <v>59</v>
       </c>
@@ -5479,7 +5478,7 @@
       </c>
       <c r="O16" s="87"/>
     </row>
-    <row r="17" spans="1:15" ht="16.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="74" t="s">
         <v>59</v>
       </c>
@@ -5547,7 +5546,7 @@
       </c>
       <c r="O18" s="87"/>
     </row>
-    <row r="19" spans="1:15" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="74" t="s">
         <v>59</v>
       </c>
@@ -5576,7 +5575,7 @@
       <c r="N19" s="143"/>
       <c r="O19" s="87"/>
     </row>
-    <row r="20" spans="1:15" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="74" t="s">
         <v>59</v>
       </c>
@@ -5607,7 +5606,7 @@
       <c r="N20" s="143"/>
       <c r="O20" s="87"/>
     </row>
-    <row r="21" spans="1:15" ht="16.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="74"/>
       <c r="B21" s="66">
         <v>7</v>
@@ -5721,18 +5720,6 @@
       <c r="O24" s="87"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H23" xr:uid="{816F3457-95CC-4A5E-96D0-1EA42C9E78DF}">
-    <filterColumn colId="4">
-      <filters>
-        <filter val="B"/>
-        <filter val="Code"/>
-        <filter val="M"/>
-        <filter val="Major"/>
-        <filter val="S"/>
-        <filter val="WIP"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <mergeCells count="2">
     <mergeCell ref="K7:L7"/>
     <mergeCell ref="K8:L8"/>
@@ -5750,8 +5737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C24F838E-581A-4053-8853-3FD311356AFD}">
   <dimension ref="B2:G60"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6124,14 +6111,14 @@
       <c r="A1" s="53"/>
       <c r="C1" s="54" t="str">
         <f ca="1">_xlfn.CONCAT("Deadline: 27-Dec | Today: ", TEXT(TODAY(),"dd-mmm"))</f>
-        <v>Deadline: 27-Dec | Today: 24-Dec</v>
+        <v>Deadline: 27-Dec | Today: 26-Dec</v>
       </c>
       <c r="D1" s="55" t="s">
         <v>96</v>
       </c>
       <c r="E1" s="56">
         <f ca="1">DATE(2024,12,27)-TODAY()-1</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -6768,14 +6755,14 @@
       <c r="A1" s="53"/>
       <c r="C1" s="54" t="str">
         <f ca="1">_xlfn.CONCAT("Deadline: 27-Dec | Today: ", TEXT(TODAY(),"dd-mmm"))</f>
-        <v>Deadline: 27-Dec | Today: 24-Dec</v>
+        <v>Deadline: 27-Dec | Today: 26-Dec</v>
       </c>
       <c r="D1" s="55" t="s">
         <v>96</v>
       </c>
       <c r="E1" s="56">
         <f ca="1">DATE(2024,12,27)-TODAY()-1</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -7375,11 +7362,11 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="166"/>
-      <c r="B8" s="168"/>
-      <c r="C8" s="170"/>
-      <c r="D8" s="172"/>
-      <c r="E8" s="174"/>
+      <c r="A8" s="175"/>
+      <c r="B8" s="176"/>
+      <c r="C8" s="177"/>
+      <c r="D8" s="178"/>
+      <c r="E8" s="179"/>
       <c r="F8" s="27" t="s">
         <v>40</v>
       </c>
@@ -7425,11 +7412,11 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="166"/>
-      <c r="B11" s="168"/>
-      <c r="C11" s="170"/>
-      <c r="D11" s="172"/>
-      <c r="E11" s="172"/>
+      <c r="A11" s="175"/>
+      <c r="B11" s="176"/>
+      <c r="C11" s="177"/>
+      <c r="D11" s="178"/>
+      <c r="E11" s="178"/>
       <c r="F11" s="21" t="s">
         <v>47</v>
       </c>
@@ -7455,11 +7442,11 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="166"/>
-      <c r="B13" s="168"/>
-      <c r="C13" s="170"/>
-      <c r="D13" s="172"/>
-      <c r="E13" s="172"/>
+      <c r="A13" s="175"/>
+      <c r="B13" s="176"/>
+      <c r="C13" s="177"/>
+      <c r="D13" s="178"/>
+      <c r="E13" s="178"/>
       <c r="F13" s="21" t="s">
         <v>51</v>
       </c>
@@ -7485,11 +7472,11 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="166"/>
-      <c r="B15" s="168"/>
-      <c r="C15" s="170"/>
-      <c r="D15" s="172"/>
-      <c r="E15" s="172"/>
+      <c r="A15" s="175"/>
+      <c r="B15" s="176"/>
+      <c r="C15" s="177"/>
+      <c r="D15" s="178"/>
+      <c r="E15" s="178"/>
       <c r="F15" s="27" t="s">
         <v>55</v>
       </c>
@@ -7515,11 +7502,11 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="175"/>
-      <c r="B17" s="176"/>
-      <c r="C17" s="177"/>
-      <c r="D17" s="178"/>
-      <c r="E17" s="179"/>
+      <c r="A17" s="166"/>
+      <c r="B17" s="168"/>
+      <c r="C17" s="170"/>
+      <c r="D17" s="172"/>
+      <c r="E17" s="174"/>
       <c r="F17" s="31" t="s">
         <v>58</v>
       </c>
@@ -7759,31 +7746,31 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="C16:C17"/>
     <mergeCell ref="D16:D17"/>
     <mergeCell ref="E16:E17"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
SA - Code for visualization
</commit_message>
<xml_diff>
--- a/Reviewer_Comments_R_1_24-Dec-2024.xlsx
+++ b/Reviewer_Comments_R_1_24-Dec-2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PhD\Publications\Research_Article_REINFORCE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BEBAB74-0291-40E9-8B90-70ACBDA75C80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B15C4A2-DCD0-494E-A0E8-E29299A8BCDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="414" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="414" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="6" r:id="rId1"/>
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="211">
   <si>
     <t>Reviewer 1</t>
   </si>
@@ -2301,9 +2301,6 @@
   </si>
   <si>
     <t>Do on single PHM-C01 or best one - simple case with NBD</t>
-  </si>
-  <si>
-    <t>Code-WIP</t>
   </si>
 </sst>
 </file>
@@ -3622,46 +3619,46 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4900,7 +4897,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{816F3457-95CC-4A5E-96D0-1EA42C9E78DF}">
   <dimension ref="A1:O24"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>
@@ -5011,8 +5008,8 @@
       <c r="D3" s="78" t="s">
         <v>109</v>
       </c>
-      <c r="E3" s="152" t="s">
-        <v>211</v>
+      <c r="E3" s="95" t="s">
+        <v>130</v>
       </c>
       <c r="F3" s="84"/>
       <c r="G3" s="84"/>
@@ -5033,11 +5030,11 @@
       </c>
       <c r="M3" s="104">
         <f>COUNTIF($E$3:$E$11,"Done")</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N3" s="105">
         <f t="shared" ref="N3" si="0">K3-M3</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O3" s="87"/>
     </row>
@@ -5115,11 +5112,11 @@
       </c>
       <c r="M5" s="157">
         <f>SUM(M2:M4)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="N5" s="109">
         <f>SUM(N2:N4)</f>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="O5" s="87"/>
     </row>
@@ -5153,11 +5150,11 @@
       </c>
       <c r="M6" s="155">
         <f>M5/$K$5</f>
-        <v>0.40909090909090912</v>
+        <v>0.45454545454545453</v>
       </c>
       <c r="N6" s="156">
         <f>N5/$K$5</f>
-        <v>0.59090909090909094</v>
+        <v>0.54545454545454541</v>
       </c>
       <c r="O6" s="87"/>
     </row>
@@ -5193,7 +5190,7 @@
       <c r="M7" s="87"/>
       <c r="N7" s="110">
         <f>(M5+L5)/K5</f>
-        <v>0.59090909090909094</v>
+        <v>0.63636363636363635</v>
       </c>
       <c r="O7" s="87" t="s">
         <v>169</v>
@@ -5737,7 +5734,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C24F838E-581A-4053-8853-3FD311356AFD}">
   <dimension ref="B2:G60"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -7362,11 +7359,11 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="175"/>
-      <c r="B8" s="176"/>
-      <c r="C8" s="177"/>
-      <c r="D8" s="178"/>
-      <c r="E8" s="179"/>
+      <c r="A8" s="166"/>
+      <c r="B8" s="168"/>
+      <c r="C8" s="170"/>
+      <c r="D8" s="172"/>
+      <c r="E8" s="174"/>
       <c r="F8" s="27" t="s">
         <v>40</v>
       </c>
@@ -7412,11 +7409,11 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="175"/>
-      <c r="B11" s="176"/>
-      <c r="C11" s="177"/>
-      <c r="D11" s="178"/>
-      <c r="E11" s="178"/>
+      <c r="A11" s="166"/>
+      <c r="B11" s="168"/>
+      <c r="C11" s="170"/>
+      <c r="D11" s="172"/>
+      <c r="E11" s="172"/>
       <c r="F11" s="21" t="s">
         <v>47</v>
       </c>
@@ -7442,11 +7439,11 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="175"/>
-      <c r="B13" s="176"/>
-      <c r="C13" s="177"/>
-      <c r="D13" s="178"/>
-      <c r="E13" s="178"/>
+      <c r="A13" s="166"/>
+      <c r="B13" s="168"/>
+      <c r="C13" s="170"/>
+      <c r="D13" s="172"/>
+      <c r="E13" s="172"/>
       <c r="F13" s="21" t="s">
         <v>51</v>
       </c>
@@ -7472,11 +7469,11 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="175"/>
-      <c r="B15" s="176"/>
-      <c r="C15" s="177"/>
-      <c r="D15" s="178"/>
-      <c r="E15" s="178"/>
+      <c r="A15" s="166"/>
+      <c r="B15" s="168"/>
+      <c r="C15" s="170"/>
+      <c r="D15" s="172"/>
+      <c r="E15" s="172"/>
       <c r="F15" s="27" t="s">
         <v>55</v>
       </c>
@@ -7502,11 +7499,11 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="166"/>
-      <c r="B17" s="168"/>
-      <c r="C17" s="170"/>
-      <c r="D17" s="172"/>
-      <c r="E17" s="174"/>
+      <c r="A17" s="175"/>
+      <c r="B17" s="176"/>
+      <c r="C17" s="177"/>
+      <c r="D17" s="178"/>
+      <c r="E17" s="179"/>
       <c r="F17" s="31" t="s">
         <v>58</v>
       </c>
@@ -7746,31 +7743,31 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="D10:D11"/>
     <mergeCell ref="E10:E11"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E16:E17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
sa code tanh study
</commit_message>
<xml_diff>
--- a/Reviewer_Comments_R_1_24-Dec-2024.xlsx
+++ b/Reviewer_Comments_R_1_24-Dec-2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PhD\Publications\Research_Article_REINFORCE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B15C4A2-DCD0-494E-A0E8-E29299A8BCDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C73988C-6E9D-4B85-B3C4-57AE4A144A9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="414" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="243">
   <si>
     <t>Reviewer 1</t>
   </si>
@@ -166,9 +166,6 @@
     <t>8. The technical contribution of this research is not adequately described in the abstract. I advise rewriting it.</t>
   </si>
   <si>
-    <t>9. The methods part is poorly designed and needs improvement to include more evidence on the adequacy of the research procedure.</t>
-  </si>
-  <si>
     <t>Reviewer 2</t>
   </si>
   <si>
@@ -1256,30 +1253,6 @@
     <t>Add confidence intervals for metrics</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Analyze/explain </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Display"/>
-        <family val="2"/>
-      </rPr>
-      <t>variability</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Display"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> in performance across datasets</t>
-    </r>
-  </si>
-  <si>
     <t>LR: Add Table. Stats of papers found and methodology employed.</t>
   </si>
   <si>
@@ -1298,9 +1271,6 @@
     <t>Discuss: Computational complexity</t>
   </si>
   <si>
-    <t>Discuss: Runtime</t>
-  </si>
-  <si>
     <t>Conclusion: Open issues for further research. </t>
   </si>
   <si>
@@ -1308,21 +1278,6 @@
   </si>
   <si>
     <t>Abstract: Technical contribution</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Methods: Add evidence + adequacy of research </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Display"/>
-        <family val="2"/>
-      </rPr>
-      <t>procedure</t>
-    </r>
   </si>
   <si>
     <t>Mention: Architectural simplicity = better performance in smaller data environments.</t>
@@ -2302,12 +2257,233 @@
   <si>
     <t>Do on single PHM-C01 or best one - simple case with NBD</t>
   </si>
+  <si>
+    <t>LR</t>
+  </si>
+  <si>
+    <t>Relu-tanh --- arch simplicity?</t>
+  </si>
+  <si>
+    <t>R-1: 1-2</t>
+  </si>
+  <si>
+    <t>R-1: 5-7</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>R-1: 2-4</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">cost-benefit analysis comparing training time to achieve precision or recall.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Show training time plot INCREASE - against increasing Recall/Pr</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Discuss: Runtime --- </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Display"/>
+        <family val="2"/>
+      </rPr>
+      <t>R1-2-3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Analyze/explain </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Aptos Display"/>
+        <family val="2"/>
+      </rPr>
+      <t>variability</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Aptos Display"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> in performance across datasets</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">9. The methods part is </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF222222"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>poorly designed</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF222222"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> and needs improvement to include more evidence on the adequacy of the research procedure.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Methods: </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Aptos Display"/>
+        <family val="2"/>
+      </rPr>
+      <t>poorly designed</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Display"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - Add evidence + adequacy of research </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Display"/>
+        <family val="2"/>
+      </rPr>
+      <t>procedure</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">R-2: 9-22
+Methods: poorly designed </t>
+  </si>
+  <si>
+    <t>- The research question
+- The theoretical framework
+- Sampling techniques
+- Design of The research
+- Methods of empirical research
+- techniques of data collection &amp; analysis
+- Reporting The findings of empirical research
+- Further information</t>
+  </si>
+  <si>
+    <t>We broadly follow the methodlogy outlined in Bouchrika2024, Germann2023, ConductER
+- Inductive approach – collect the data, then develop the theory.
+research gap, research questions, and research strategy
+First, confirmatory research (also deductive research) uses existing theories to derive the hypothesis (Hurley et al., 1997, p. 672). Based on a natural science perspective, confirmatory research starts with the general and progresses to the specific. Exploratory research (also inductive research) follows a reverse rationale to confirmatory research (Jaeger &amp; Halliday, 1998, p. 64). It is based on the human science view and starts from the observation of specific patterns in order to conclude analogous research findings.
+Second, a quantitative approach has traditionally been the predominant approach in research. This approach is used to validate existing theories through statistical measures (confirmatory research). Its key strength is the statistical objectivity of the results.
+Research Design</t>
+  </si>
+  <si>
+    <t>R-1: 5-8</t>
+  </si>
+  <si>
+    <t>Technique Use-case Problem type Dataset used Classification</t>
+  </si>
+  <si>
+    <t>accuracy</t>
+  </si>
+  <si>
+    <t>R2% MAE RMSE Model size</t>
+  </si>
+  <si>
+    <t>(kB)</t>
+  </si>
+  <si>
+    <t>CNN with Attention</t>
+  </si>
+  <si>
+    <t>Knowledge Distillation</t>
+  </si>
+  <si>
+    <t>[ 12 ]</t>
+  </si>
+  <si>
+    <t>Bearings: Classification</t>
+  </si>
+  <si>
+    <t>of faults</t>
+  </si>
+  <si>
+    <t>1-D time-series signal</t>
+  </si>
+  <si>
+    <t>(univariate)</t>
+  </si>
+  <si>
+    <t>Case Western Reserve</t>
+  </si>
+  <si>
+    <t>University [ 47 ]</t>
+  </si>
+  <si>
+    <t>97.2 % NA NA NA 192.0</t>
+  </si>
+  <si>
+    <t>CNN based LeNet [ 16 ] Bearings: Classification</t>
+  </si>
+  <si>
+    <t>IEEE PHM Challenge</t>
+  </si>
+  <si>
+    <t>(2012) [ 48 ]</t>
+  </si>
+  <si>
+    <t>95.3 % NA NA NA 17.0</t>
+  </si>
+  <si>
+    <t>Patange2021Review, Siraskar2024NW</t>
+  </si>
+  <si>
+    <t>Siraskar - conducts ML analysis on the same dataset PHM and ….</t>
+  </si>
+  <si>
+    <t>Patange2021Review, notice that SVM is most common classiifer for faults with 4 of 8 50% and 90.8 to 96.7 range accuracy , NB-1, tree-1, knearnts-1, clab</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="57" x14ac:knownFonts="1">
+  <fonts count="61" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2699,6 +2875,36 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Display"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Aptos Display"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="15">
@@ -3134,7 +3340,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="39" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="180">
+  <cellXfs count="186">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -3610,7 +3816,25 @@
     <xf numFmtId="0" fontId="31" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="16" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -3619,46 +3843,46 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4629,6 +4853,94 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1767167</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>171041</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>234182</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>101557</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C159438D-B21C-FFD6-EFB2-5722DDFE5346}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2376767" y="29565191"/>
+          <a:ext cx="9344565" cy="3359516"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>296575</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>152673</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{94CD26F4-E92B-BDDB-2874-8F129CC22DEB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2466975" y="27784425"/>
+          <a:ext cx="9316750" cy="1952898"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4897,20 +5209,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{816F3457-95CC-4A5E-96D0-1EA42C9E78DF}">
   <dimension ref="A1:O24"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomLeft" activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" style="71" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="2.140625" style="71" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="83.28515625" style="62" customWidth="1"/>
+    <col min="3" max="3" width="3.28515625" style="51" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="66.42578125" style="62" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" style="82" customWidth="1"/>
     <col min="6" max="7" width="6.140625" style="82" customWidth="1"/>
-    <col min="8" max="8" width="60.5703125" style="82" customWidth="1"/>
+    <col min="8" max="8" width="41" style="82" customWidth="1"/>
     <col min="9" max="9" width="2.28515625" style="62" customWidth="1"/>
     <col min="10" max="10" width="9" style="62" customWidth="1"/>
     <col min="11" max="13" width="5.85546875" style="62" customWidth="1"/>
@@ -4922,64 +5234,66 @@
     <row r="1" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="72"/>
       <c r="B1" s="63"/>
-      <c r="C1" s="9"/>
+      <c r="C1" s="167"/>
       <c r="D1" s="77" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E1" s="115" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="F1" s="115" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="G1" s="115" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="H1" s="116" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="I1" s="86"/>
       <c r="J1" s="123" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="K1" s="124" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L1" s="124" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M1" s="124" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="N1" s="103" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="O1" s="86"/>
     </row>
     <row r="2" spans="1:15" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="73" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B2" s="64">
         <v>1</v>
       </c>
-      <c r="C2" s="41">
+      <c r="C2" s="42">
         <v>1</v>
       </c>
       <c r="D2" s="61" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="E2" s="99" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="F2" s="99" t="s">
-        <v>130</v>
-      </c>
-      <c r="G2" s="61"/>
+        <v>126</v>
+      </c>
+      <c r="G2" s="61" t="s">
+        <v>211</v>
+      </c>
       <c r="H2" s="117"/>
       <c r="I2" s="87"/>
       <c r="J2" s="125" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="K2" s="104">
         <f>COUNTA(C2)</f>
@@ -4997,28 +5311,32 @@
     </row>
     <row r="3" spans="1:15" ht="16.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="74" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" s="65">
         <v>1</v>
       </c>
-      <c r="C3" s="18">
+      <c r="C3" s="28">
         <v>2</v>
       </c>
       <c r="D3" s="78" t="s">
-        <v>109</v>
-      </c>
-      <c r="E3" s="95" t="s">
-        <v>130</v>
-      </c>
-      <c r="F3" s="84"/>
-      <c r="G3" s="84"/>
+        <v>108</v>
+      </c>
+      <c r="E3" s="152" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="84" t="s">
+        <v>211</v>
+      </c>
+      <c r="G3" s="84" t="s">
+        <v>211</v>
+      </c>
       <c r="H3" s="118" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="I3" s="87"/>
       <c r="J3" s="126" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K3" s="104">
         <f>COUNTA(C3:C11)</f>
@@ -5026,42 +5344,46 @@
       </c>
       <c r="L3" s="104">
         <f>COUNTIF($E$3:$E$11,"WIP")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M3" s="104">
         <f>COUNTIF($E$3:$E$11,"Done")</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N3" s="105">
         <f t="shared" ref="N3" si="0">K3-M3</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="O3" s="87"/>
     </row>
     <row r="4" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="74" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4" s="66">
         <v>2</v>
       </c>
-      <c r="C4" s="18">
+      <c r="C4" s="28">
         <v>3</v>
       </c>
       <c r="D4" s="78" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E4" s="95" t="s">
-        <v>130</v>
-      </c>
-      <c r="F4" s="84"/>
-      <c r="G4" s="84"/>
+        <v>126</v>
+      </c>
+      <c r="F4" s="84" t="s">
+        <v>211</v>
+      </c>
+      <c r="G4" s="84" t="s">
+        <v>211</v>
+      </c>
       <c r="H4" s="118" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="I4" s="87"/>
       <c r="J4" s="127" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K4" s="106">
         <f>COUNTA(C12:C23)</f>
@@ -5073,11 +5395,11 @@
       </c>
       <c r="M4" s="106">
         <f>COUNTIF($E$12:$E$23,"Done")</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="N4" s="107">
         <f>K4-M4</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="O4" s="87"/>
     </row>
@@ -5086,19 +5408,23 @@
       <c r="B5" s="66">
         <v>2</v>
       </c>
-      <c r="C5" s="18">
+      <c r="C5" s="28">
         <v>4</v>
       </c>
       <c r="D5" s="78" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E5" s="160" t="s">
-        <v>38</v>
-      </c>
-      <c r="F5" s="84"/>
-      <c r="G5" s="84"/>
+        <v>37</v>
+      </c>
+      <c r="F5" s="84" t="s">
+        <v>211</v>
+      </c>
+      <c r="G5" s="84" t="s">
+        <v>211</v>
+      </c>
       <c r="H5" s="118" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="I5" s="87"/>
       <c r="J5" s="88"/>
@@ -5108,7 +5434,7 @@
       </c>
       <c r="L5" s="108">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M5" s="157">
         <f>SUM(M2:M4)</f>
@@ -5122,31 +5448,35 @@
     </row>
     <row r="6" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="74" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6" s="65">
         <v>3</v>
       </c>
-      <c r="C6" s="18">
+      <c r="C6" s="28">
         <v>5</v>
       </c>
       <c r="D6" s="78" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E6" s="161" t="s">
-        <v>44</v>
-      </c>
-      <c r="F6" s="84"/>
-      <c r="G6" s="84"/>
+        <v>43</v>
+      </c>
+      <c r="F6" s="84" t="s">
+        <v>211</v>
+      </c>
+      <c r="G6" s="84" t="s">
+        <v>211</v>
+      </c>
       <c r="H6" s="118" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="I6" s="87"/>
       <c r="J6" s="153"/>
       <c r="K6" s="153"/>
       <c r="L6" s="154">
         <f>L5/$K$5</f>
-        <v>0.18181818181818182</v>
+        <v>0.22727272727272727</v>
       </c>
       <c r="M6" s="155">
         <f>M5/$K$5</f>
@@ -5160,70 +5490,78 @@
     </row>
     <row r="7" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="74" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" s="65">
         <v>4</v>
       </c>
-      <c r="C7" s="18">
+      <c r="C7" s="28">
         <v>6</v>
       </c>
       <c r="D7" s="78" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E7" s="95" t="s">
-        <v>130</v>
-      </c>
-      <c r="F7" s="84"/>
-      <c r="G7" s="84"/>
+        <v>126</v>
+      </c>
+      <c r="F7" s="84" t="s">
+        <v>211</v>
+      </c>
+      <c r="G7" s="84" t="s">
+        <v>211</v>
+      </c>
       <c r="H7" s="118" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="I7" s="87"/>
       <c r="J7" s="101" t="s">
-        <v>131</v>
-      </c>
-      <c r="K7" s="164">
+        <v>127</v>
+      </c>
+      <c r="K7" s="170">
         <v>45657</v>
       </c>
-      <c r="L7" s="164"/>
+      <c r="L7" s="170"/>
       <c r="M7" s="87"/>
       <c r="N7" s="110">
         <f>(M5+L5)/K5</f>
-        <v>0.63636363636363635</v>
+        <v>0.68181818181818177</v>
       </c>
       <c r="O7" s="87" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="74" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" s="66">
         <v>5</v>
       </c>
-      <c r="C8" s="18">
+      <c r="C8" s="28">
         <v>7</v>
       </c>
       <c r="D8" s="78" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E8" s="152" t="s">
-        <v>34</v>
-      </c>
-      <c r="F8" s="84"/>
-      <c r="G8" s="84"/>
+        <v>33</v>
+      </c>
+      <c r="F8" s="84" t="s">
+        <v>211</v>
+      </c>
+      <c r="G8" s="84" t="s">
+        <v>211</v>
+      </c>
       <c r="H8" s="118"/>
       <c r="I8" s="87"/>
       <c r="J8" s="101" t="s">
-        <v>132</v>
-      </c>
-      <c r="K8" s="164">
+        <v>128</v>
+      </c>
+      <c r="K8" s="170">
         <f ca="1">TODAY()</f>
         <v>45652</v>
       </c>
-      <c r="L8" s="164"/>
+      <c r="L8" s="170"/>
       <c r="M8" s="87"/>
       <c r="N8" s="87"/>
       <c r="O8" s="87"/>
@@ -5233,23 +5571,27 @@
       <c r="B9" s="66">
         <v>5</v>
       </c>
-      <c r="C9" s="18">
+      <c r="C9" s="165">
         <v>8</v>
       </c>
-      <c r="D9" s="78" t="s">
-        <v>125</v>
+      <c r="D9" s="163" t="s">
+        <v>121</v>
       </c>
       <c r="E9" s="152" t="s">
-        <v>34</v>
-      </c>
-      <c r="F9" s="84"/>
-      <c r="G9" s="84"/>
+        <v>33</v>
+      </c>
+      <c r="F9" s="84" t="s">
+        <v>211</v>
+      </c>
+      <c r="G9" s="84" t="s">
+        <v>211</v>
+      </c>
       <c r="H9" s="118" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="I9" s="87"/>
       <c r="J9" s="101" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K9" s="87">
         <f ca="1">K7-K8-1</f>
@@ -5262,24 +5604,28 @@
     </row>
     <row r="10" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="74" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B10" s="67">
         <v>6</v>
       </c>
-      <c r="C10" s="18">
+      <c r="C10" s="28">
         <v>9</v>
       </c>
       <c r="D10" s="78" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E10" s="95" t="s">
-        <v>130</v>
-      </c>
-      <c r="F10" s="89"/>
-      <c r="G10" s="89"/>
+        <v>126</v>
+      </c>
+      <c r="F10" s="89" t="s">
+        <v>211</v>
+      </c>
+      <c r="G10" s="89" t="s">
+        <v>211</v>
+      </c>
       <c r="H10" s="119" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="I10" s="87"/>
       <c r="J10" s="87"/>
@@ -5294,17 +5640,21 @@
       <c r="B11" s="68">
         <v>6</v>
       </c>
-      <c r="C11" s="46">
+      <c r="C11" s="166">
         <v>10</v>
       </c>
-      <c r="D11" s="79" t="s">
-        <v>112</v>
+      <c r="D11" s="164" t="s">
+        <v>215</v>
       </c>
       <c r="E11" s="162" t="s">
-        <v>195</v>
-      </c>
-      <c r="F11" s="85"/>
-      <c r="G11" s="85"/>
+        <v>191</v>
+      </c>
+      <c r="F11" s="85" t="s">
+        <v>211</v>
+      </c>
+      <c r="G11" s="85" t="s">
+        <v>211</v>
+      </c>
       <c r="H11" s="120"/>
       <c r="I11" s="87"/>
       <c r="J11" s="87"/>
@@ -5316,63 +5666,71 @@
     </row>
     <row r="12" spans="1:15" ht="16.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A12" s="74" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B12" s="65">
         <v>1</v>
       </c>
-      <c r="C12" s="18">
+      <c r="C12" s="28">
         <v>11</v>
       </c>
       <c r="D12" s="78" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E12" s="161" t="s">
-        <v>37</v>
-      </c>
-      <c r="F12" s="84"/>
-      <c r="G12" s="84"/>
+        <v>36</v>
+      </c>
+      <c r="F12" s="84" t="s">
+        <v>211</v>
+      </c>
+      <c r="G12" s="84" t="s">
+        <v>211</v>
+      </c>
       <c r="H12" s="118"/>
       <c r="I12" s="87"/>
       <c r="J12" s="139" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="K12" s="140" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L12" s="140" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M12" s="140" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="N12" s="141" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="O12" s="87"/>
     </row>
     <row r="13" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="74" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B13" s="66">
         <v>2</v>
       </c>
-      <c r="C13" s="18">
+      <c r="C13" s="28">
         <v>12</v>
       </c>
       <c r="D13" s="78" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E13" s="161" t="s">
-        <v>104</v>
-      </c>
-      <c r="F13" s="84"/>
-      <c r="G13" s="84"/>
+        <v>103</v>
+      </c>
+      <c r="F13" s="84" t="s">
+        <v>211</v>
+      </c>
+      <c r="G13" s="84" t="s">
+        <v>211</v>
+      </c>
       <c r="H13" s="118"/>
       <c r="I13" s="87"/>
       <c r="J13" s="142" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="K13" s="136"/>
       <c r="L13" s="136"/>
@@ -5385,23 +5743,27 @@
       <c r="B14" s="66">
         <v>2</v>
       </c>
-      <c r="C14" s="18">
+      <c r="C14" s="28">
         <v>13</v>
       </c>
       <c r="D14" s="78" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E14" s="95" t="s">
-        <v>130</v>
-      </c>
-      <c r="F14" s="84"/>
-      <c r="G14" s="84"/>
+        <v>126</v>
+      </c>
+      <c r="F14" s="84" t="s">
+        <v>211</v>
+      </c>
+      <c r="G14" s="84" t="s">
+        <v>211</v>
+      </c>
       <c r="H14" s="118" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="I14" s="87"/>
       <c r="J14" s="144" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K14" s="136"/>
       <c r="L14" s="136"/>
@@ -5414,21 +5776,25 @@
       <c r="B15" s="66">
         <v>2</v>
       </c>
-      <c r="C15" s="18">
+      <c r="C15" s="28">
         <v>14</v>
       </c>
       <c r="D15" s="78" t="s">
-        <v>119</v>
+        <v>214</v>
       </c>
       <c r="E15" s="152" t="s">
-        <v>34</v>
-      </c>
-      <c r="F15" s="84"/>
-      <c r="G15" s="84"/>
+        <v>33</v>
+      </c>
+      <c r="F15" s="84" t="s">
+        <v>211</v>
+      </c>
+      <c r="G15" s="84" t="s">
+        <v>211</v>
+      </c>
       <c r="H15" s="118"/>
       <c r="I15" s="87"/>
       <c r="J15" s="146" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K15" s="147"/>
       <c r="L15" s="147"/>
@@ -5438,22 +5804,26 @@
     </row>
     <row r="16" spans="1:15" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="74" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B16" s="65">
         <v>3</v>
       </c>
-      <c r="C16" s="18">
+      <c r="C16" s="28">
         <v>15</v>
       </c>
       <c r="D16" s="78" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E16" s="95" t="s">
-        <v>130</v>
-      </c>
-      <c r="F16" s="84"/>
-      <c r="G16" s="84"/>
+        <v>126</v>
+      </c>
+      <c r="F16" s="84" t="s">
+        <v>211</v>
+      </c>
+      <c r="G16" s="84" t="s">
+        <v>211</v>
+      </c>
       <c r="H16" s="118"/>
       <c r="I16" s="87"/>
       <c r="J16" s="149"/>
@@ -5477,24 +5847,28 @@
     </row>
     <row r="17" spans="1:15" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="74" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B17" s="65">
         <v>4</v>
       </c>
-      <c r="C17" s="18">
+      <c r="C17" s="28">
         <v>16</v>
       </c>
       <c r="D17" s="78" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E17" s="95" t="s">
-        <v>130</v>
-      </c>
-      <c r="F17" s="83"/>
-      <c r="G17" s="83"/>
+        <v>126</v>
+      </c>
+      <c r="F17" s="83" t="s">
+        <v>211</v>
+      </c>
+      <c r="G17" s="84" t="s">
+        <v>211</v>
+      </c>
       <c r="H17" s="121" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="I17" s="87"/>
       <c r="J17" s="137"/>
@@ -5506,65 +5880,73 @@
     </row>
     <row r="18" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="74" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B18" s="65">
         <v>5</v>
       </c>
-      <c r="C18" s="18">
+      <c r="C18" s="28">
         <v>17</v>
       </c>
       <c r="D18" s="78" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E18" s="152" t="s">
-        <v>34</v>
-      </c>
-      <c r="F18" s="84"/>
-      <c r="G18" s="84"/>
+        <v>33</v>
+      </c>
+      <c r="F18" s="84" t="s">
+        <v>211</v>
+      </c>
+      <c r="G18" s="84" t="s">
+        <v>211</v>
+      </c>
       <c r="H18" s="118" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="I18" s="87"/>
       <c r="J18" s="145" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="K18" s="140" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L18" s="140" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M18" s="140" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="N18" s="141" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="O18" s="87"/>
     </row>
     <row r="19" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="74" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B19" s="65">
         <v>6</v>
       </c>
-      <c r="C19" s="18">
+      <c r="C19" s="28">
         <v>18</v>
       </c>
       <c r="D19" s="78" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E19" s="161" t="s">
-        <v>104</v>
-      </c>
-      <c r="F19" s="84"/>
-      <c r="G19" s="84"/>
+        <v>103</v>
+      </c>
+      <c r="F19" s="84" t="s">
+        <v>211</v>
+      </c>
+      <c r="G19" s="84" t="s">
+        <v>211</v>
+      </c>
       <c r="H19" s="118"/>
       <c r="I19" s="87"/>
       <c r="J19" s="142" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="K19" s="136"/>
       <c r="L19" s="136"/>
@@ -5574,28 +5956,32 @@
     </row>
     <row r="20" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="74" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B20" s="66">
         <v>7</v>
       </c>
-      <c r="C20" s="18">
+      <c r="C20" s="28">
         <v>19</v>
       </c>
       <c r="D20" s="78" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E20" s="95" t="s">
-        <v>130</v>
-      </c>
-      <c r="F20" s="84"/>
-      <c r="G20" s="84"/>
+        <v>126</v>
+      </c>
+      <c r="F20" s="84" t="s">
+        <v>211</v>
+      </c>
+      <c r="G20" s="84" t="s">
+        <v>211</v>
+      </c>
       <c r="H20" s="118" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="I20" s="87"/>
       <c r="J20" s="144" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K20" s="136"/>
       <c r="L20" s="136"/>
@@ -5608,25 +5994,27 @@
       <c r="B21" s="66">
         <v>7</v>
       </c>
-      <c r="C21" s="18">
+      <c r="C21" s="28">
         <v>20</v>
       </c>
       <c r="D21" s="78" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E21" s="95" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="F21" s="84" t="s">
-        <v>163</v>
-      </c>
-      <c r="G21" s="84"/>
+        <v>159</v>
+      </c>
+      <c r="G21" s="84" t="s">
+        <v>211</v>
+      </c>
       <c r="H21" s="118" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="I21" s="87"/>
       <c r="J21" s="146" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K21" s="147"/>
       <c r="L21" s="147"/>
@@ -5636,22 +6024,26 @@
     </row>
     <row r="22" spans="1:15" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="74" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B22" s="65">
         <v>8</v>
       </c>
-      <c r="C22" s="18">
+      <c r="C22" s="28">
         <v>21</v>
       </c>
       <c r="D22" s="78" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E22" s="161" t="s">
-        <v>104</v>
-      </c>
-      <c r="F22" s="84"/>
-      <c r="G22" s="84"/>
+        <v>103</v>
+      </c>
+      <c r="F22" s="84" t="s">
+        <v>211</v>
+      </c>
+      <c r="G22" s="84" t="s">
+        <v>211</v>
+      </c>
       <c r="H22" s="118"/>
       <c r="I22" s="87"/>
       <c r="J22" s="149"/>
@@ -5675,22 +6067,26 @@
     </row>
     <row r="23" spans="1:15" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="75" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B23" s="69">
         <v>9</v>
       </c>
-      <c r="C23" s="46">
+      <c r="C23" s="166">
         <v>22</v>
       </c>
       <c r="D23" s="79" t="s">
-        <v>123</v>
-      </c>
-      <c r="E23" s="163" t="s">
-        <v>44</v>
-      </c>
-      <c r="F23" s="85"/>
-      <c r="G23" s="85"/>
+        <v>217</v>
+      </c>
+      <c r="E23" s="169" t="s">
+        <v>126</v>
+      </c>
+      <c r="F23" s="85" t="s">
+        <v>211</v>
+      </c>
+      <c r="G23" s="85" t="s">
+        <v>211</v>
+      </c>
       <c r="H23" s="120"/>
       <c r="I23" s="87"/>
       <c r="J23" s="87"/>
@@ -5703,7 +6099,7 @@
     <row r="24" spans="1:15" ht="16.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A24" s="76"/>
       <c r="B24" s="70"/>
-      <c r="C24" s="32"/>
+      <c r="C24" s="25"/>
       <c r="D24" s="80"/>
       <c r="E24" s="81"/>
       <c r="F24" s="81"/>
@@ -5732,10 +6128,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C24F838E-581A-4053-8853-3FD311356AFD}">
-  <dimension ref="B2:G60"/>
+  <dimension ref="B2:H92"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5748,19 +6144,19 @@
   <sheetData>
     <row r="2" spans="2:5" ht="21" x14ac:dyDescent="0.25">
       <c r="B2" s="112" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C2" s="112"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="90" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C4" s="92" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="D4" s="91" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
@@ -5768,21 +6164,21 @@
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="90" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C6" s="92" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D6" s="100" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E6" s="100" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C7" s="92" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="D7">
         <v>2024</v>
@@ -5793,7 +6189,7 @@
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C8" s="92" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D8">
         <v>2023</v>
@@ -5804,7 +6200,7 @@
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C9" s="92" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D9">
         <v>2022</v>
@@ -5815,7 +6211,7 @@
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="94" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D10">
         <v>2021</v>
@@ -5826,7 +6222,7 @@
     </row>
     <row r="11" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C11" s="93" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D11">
         <v>2020</v>
@@ -5840,10 +6236,10 @@
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" s="90" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C13" s="111" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D13">
         <v>2019</v>
@@ -5854,26 +6250,26 @@
     </row>
     <row r="14" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B14" s="93" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C14" s="93" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="15" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B15" s="92" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C15" s="93" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="16" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B16" s="114" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C16" s="113" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D16" s="18"/>
       <c r="E16" s="78"/>
@@ -5881,20 +6277,20 @@
     <row r="18" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B18" s="111"/>
       <c r="C18" s="93" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="20" spans="2:7" ht="195" x14ac:dyDescent="0.25">
       <c r="B20" s="90" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C20" s="93" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="21" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="C21" s="93" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="F21" s="66">
         <v>2</v>
@@ -5905,54 +6301,54 @@
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="92" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C26" s="92" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C27" s="92" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C28" s="92" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C29" s="92" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="31" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B31" s="128" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C31" s="129" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="D31" s="130"/>
     </row>
     <row r="32" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="C32" s="93" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="33" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="C33" s="93" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="34" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="C34" s="93" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
     <row r="35" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="C35" s="93" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.25">
@@ -5962,117 +6358,300 @@
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B38" s="128" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C38" s="134" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D38" s="130"/>
       <c r="E38" s="130"/>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C39" s="92" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C40" s="92" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B41" s="135"/>
       <c r="C41" s="132" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="D41" s="133"/>
       <c r="E41" s="133"/>
     </row>
     <row r="43" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B43" s="128" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C43" s="134" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="44" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C44" s="93" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="46" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B46" s="134" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C46" s="134" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="47" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="C47" s="93" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="49" spans="2:3" ht="60" x14ac:dyDescent="0.25">
       <c r="B49" s="131" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C49" s="132" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B51" s="92" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C51" s="158" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="52" spans="2:3" ht="60" x14ac:dyDescent="0.25">
       <c r="B52" s="78" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C52" s="93" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C53" s="92" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C54" s="92" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="55" spans="2:3" ht="75" x14ac:dyDescent="0.25">
       <c r="C55" s="93" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="57" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B57" s="92" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C57" s="159" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C58" s="92" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B59" s="131"/>
+      <c r="C59" s="132" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B60" s="92" t="s">
+        <v>209</v>
+      </c>
+      <c r="C60" s="92" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B61" s="131" t="s">
+        <v>210</v>
+      </c>
+      <c r="C61" s="131" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="59" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="C59" s="93" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C60" s="93"/>
+    <row r="62" spans="2:3" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B62" s="92" t="s">
+        <v>212</v>
+      </c>
+      <c r="C62" s="114" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="63" spans="2:3" ht="180" x14ac:dyDescent="0.25">
+      <c r="B63" s="93" t="s">
+        <v>218</v>
+      </c>
+      <c r="C63" s="93" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="64" spans="2:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="C64" s="168" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E65" s="74" t="s">
+        <v>22</v>
+      </c>
+      <c r="F65" s="65">
+        <v>1</v>
+      </c>
+      <c r="G65" s="18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B66" s="92" t="s">
+        <v>221</v>
+      </c>
+      <c r="C66" s="163" t="s">
+        <v>121</v>
+      </c>
+      <c r="E66" s="74" t="s">
+        <v>22</v>
+      </c>
+      <c r="F66" s="66">
+        <v>5</v>
+      </c>
+      <c r="G66" s="18">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C67" s="92" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C68" s="92" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C69" s="92" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H72" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="73" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H73" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="74" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H74" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="75" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H75" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="76" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H76" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="77" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H77" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="78" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H78" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="79" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H79" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="80" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H80" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="81" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H81" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="82" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H82" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="83" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H83" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="84" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H84" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="85" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H85" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="86" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H86" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="87" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H87" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="88" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H88" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="89" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H89" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="90" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H90" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="91" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H91" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="92" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H92" t="s">
+        <v>239</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6111,7 +6690,7 @@
         <v>Deadline: 27-Dec | Today: 26-Dec</v>
       </c>
       <c r="D1" s="55" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E1" s="56">
         <f ca="1">DATE(2024,12,27)-TODAY()-1</f>
@@ -6122,36 +6701,36 @@
       <c r="A2" s="8"/>
       <c r="B2" s="9"/>
       <c r="C2" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="43" t="s">
+      <c r="E2" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="10" t="s">
-        <v>26</v>
-      </c>
       <c r="F2" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H2" s="50" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I2" s="51">
         <f>COUNTIF($D$4:$D$9, "Done")</f>
         <v>0</v>
       </c>
       <c r="J2" s="50" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K2" s="51">
         <f>COUNTIF($D$10:$D$18, "Done")</f>
         <v>0</v>
       </c>
       <c r="L2" s="50" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="M2" s="51">
         <v>1</v>
@@ -6159,26 +6738,26 @@
     </row>
     <row r="3" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="40" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3" s="41">
         <v>1</v>
       </c>
       <c r="C3" s="59" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="44" t="s">
+      <c r="E3" s="42" t="s">
         <v>34</v>
-      </c>
-      <c r="E3" s="42" t="s">
-        <v>35</v>
       </c>
       <c r="F3" s="42"/>
       <c r="G3" s="58" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H3" s="52" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I3" s="7">
         <f>COUNTA($D$4:$D$9)</f>
@@ -6194,325 +6773,325 @@
     </row>
     <row r="4" spans="1:13" ht="60.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4" s="18">
         <v>1</v>
       </c>
       <c r="C4" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="28" t="s">
+      <c r="E4" s="28" t="s">
         <v>37</v>
-      </c>
-      <c r="E4" s="28" t="s">
-        <v>38</v>
       </c>
       <c r="F4" s="28"/>
       <c r="G4" s="27" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" s="18">
         <v>2</v>
       </c>
       <c r="C5" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="G5" s="27" t="s">
         <v>41</v>
-      </c>
-      <c r="D5" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="E5" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="F5" s="28" t="s">
-        <v>98</v>
-      </c>
-      <c r="G5" s="27" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6" s="18">
         <v>3</v>
       </c>
       <c r="C6" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="D6" s="28" t="s">
+      <c r="E6" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="E6" s="28" t="s">
-        <v>45</v>
-      </c>
       <c r="F6" s="28" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G6" s="27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" s="18">
         <v>4</v>
       </c>
       <c r="C7" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="28" t="s">
         <v>48</v>
-      </c>
-      <c r="D7" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="E7" s="28" t="s">
-        <v>49</v>
       </c>
       <c r="F7" s="28"/>
       <c r="G7" s="27" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" s="18">
         <v>5</v>
       </c>
       <c r="C8" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="D8" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="E8" s="28" t="s">
-        <v>53</v>
-      </c>
       <c r="F8" s="28" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G8" s="27" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="45" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" s="46">
         <v>6</v>
       </c>
       <c r="C9" s="47" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D9" s="48" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="48" t="s">
         <v>37</v>
-      </c>
-      <c r="E9" s="48" t="s">
-        <v>38</v>
       </c>
       <c r="F9" s="48"/>
       <c r="G9" s="57" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="60.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B10" s="18">
         <v>1</v>
       </c>
       <c r="C10" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="D10" s="28" t="s">
+      <c r="E10" s="28" t="s">
         <v>61</v>
-      </c>
-      <c r="E10" s="28" t="s">
-        <v>62</v>
       </c>
       <c r="F10" s="28"/>
       <c r="G10" s="27" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B11" s="18">
         <v>2</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D11" s="28" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E11" s="28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F11" s="28"/>
       <c r="G11" s="27" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B12" s="18">
         <v>3</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D12" s="28" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E12" s="28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F12" s="28"/>
       <c r="G12" s="27" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B13" s="18">
         <v>4</v>
       </c>
       <c r="C13" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="D13" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="E13" s="28" t="s">
+      <c r="F13" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="G13" s="27" t="s">
         <v>69</v>
-      </c>
-      <c r="F13" s="28" t="s">
-        <v>97</v>
-      </c>
-      <c r="G13" s="27" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B14" s="18">
         <v>5</v>
       </c>
       <c r="C14" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="D14" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" s="28" t="s">
         <v>71</v>
-      </c>
-      <c r="D14" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="E14" s="28" t="s">
-        <v>72</v>
       </c>
       <c r="F14" s="28"/>
       <c r="G14" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B15" s="18">
         <v>6</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D15" s="28" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E15" s="28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F15" s="28"/>
       <c r="G15" s="21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B16" s="18">
         <v>7</v>
       </c>
       <c r="C16" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="D16" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="28" t="s">
         <v>76</v>
-      </c>
-      <c r="D16" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="E16" s="28" t="s">
-        <v>77</v>
       </c>
       <c r="F16" s="28"/>
       <c r="G16" s="21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B17" s="18">
         <v>8</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D17" s="28" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E17" s="28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F17" s="28"/>
       <c r="G17" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="45" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B18" s="46">
         <v>9</v>
       </c>
       <c r="C18" s="47" t="s">
+        <v>80</v>
+      </c>
+      <c r="D18" s="48" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" s="48" t="s">
         <v>81</v>
-      </c>
-      <c r="D18" s="48" t="s">
-        <v>44</v>
-      </c>
-      <c r="E18" s="48" t="s">
-        <v>82</v>
       </c>
       <c r="F18" s="48"/>
       <c r="G18" s="49" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -6528,7 +7107,7 @@
       <c r="A20" s="24"/>
       <c r="B20" s="32"/>
       <c r="C20" s="34" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D20" s="25"/>
       <c r="E20" s="25"/>
@@ -6539,7 +7118,7 @@
       <c r="A21" s="24"/>
       <c r="B21" s="32"/>
       <c r="C21" s="35" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D21" s="25">
         <v>79</v>
@@ -6552,7 +7131,7 @@
       <c r="A22" s="24"/>
       <c r="B22" s="32"/>
       <c r="C22" s="35" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D22" s="25">
         <v>103</v>
@@ -6565,7 +7144,7 @@
       <c r="A23" s="36"/>
       <c r="B23" s="37"/>
       <c r="C23" s="38" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D23" s="39">
         <v>118</v>
@@ -6583,8 +7162,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B55CCE9F-712C-4507-AED0-56401ED0B51C}">
   <dimension ref="B1:D25"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6595,12 +7174,12 @@
   <sheetData>
     <row r="1" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B1" s="96" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B2" s="97" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
@@ -6608,7 +7187,7 @@
         <v>0</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="57" x14ac:dyDescent="0.25">
@@ -6676,7 +7255,7 @@
     <row r="15" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="D15" s="5" t="s">
-        <v>21</v>
+        <v>216</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="42.75" x14ac:dyDescent="0.25">
@@ -6730,7 +7309,7 @@
   <dimension ref="A1:M23"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -6755,7 +7334,7 @@
         <v>Deadline: 27-Dec | Today: 26-Dec</v>
       </c>
       <c r="D1" s="55" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E1" s="56">
         <f ca="1">DATE(2024,12,27)-TODAY()-1</f>
@@ -6766,36 +7345,36 @@
       <c r="A2" s="8"/>
       <c r="B2" s="9"/>
       <c r="C2" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="43" t="s">
+      <c r="E2" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="10" t="s">
-        <v>26</v>
-      </c>
       <c r="F2" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H2" s="50" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I2" s="51">
         <f>COUNTIF($D$4:$D$9, "Done")</f>
         <v>0</v>
       </c>
       <c r="J2" s="50" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K2" s="51">
         <f>COUNTIF($D$10:$D$18, "Done")</f>
         <v>0</v>
       </c>
       <c r="L2" s="50" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="M2" s="51">
         <v>1</v>
@@ -6803,26 +7382,26 @@
     </row>
     <row r="3" spans="1:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="40" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3" s="41">
         <v>1</v>
       </c>
       <c r="C3" s="98" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="44" t="s">
+      <c r="E3" s="42" t="s">
         <v>34</v>
-      </c>
-      <c r="E3" s="42" t="s">
-        <v>35</v>
       </c>
       <c r="F3" s="42"/>
       <c r="G3" s="58" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H3" s="52" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I3" s="7">
         <f>COUNTA($D$4:$D$9)</f>
@@ -6838,325 +7417,325 @@
     </row>
     <row r="4" spans="1:13" ht="60.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4" s="18">
         <v>1</v>
       </c>
       <c r="C4" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="28" t="s">
+      <c r="E4" s="60" t="s">
         <v>37</v>
-      </c>
-      <c r="E4" s="60" t="s">
-        <v>38</v>
       </c>
       <c r="F4" s="28"/>
       <c r="G4" s="27" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" s="18">
         <v>2</v>
       </c>
       <c r="C5" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="G5" s="27" t="s">
         <v>41</v>
-      </c>
-      <c r="D5" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="E5" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="F5" s="28" t="s">
-        <v>98</v>
-      </c>
-      <c r="G5" s="27" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6" s="18">
         <v>3</v>
       </c>
       <c r="C6" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="D6" s="28" t="s">
+      <c r="E6" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="E6" s="28" t="s">
-        <v>45</v>
-      </c>
       <c r="F6" s="28" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G6" s="27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" s="18">
         <v>4</v>
       </c>
       <c r="C7" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="28" t="s">
         <v>48</v>
-      </c>
-      <c r="D7" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="E7" s="28" t="s">
-        <v>49</v>
       </c>
       <c r="F7" s="28"/>
       <c r="G7" s="27" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" s="18">
         <v>5</v>
       </c>
       <c r="C8" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="D8" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="E8" s="28" t="s">
-        <v>53</v>
-      </c>
       <c r="F8" s="28" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G8" s="27" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="45" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" s="46">
         <v>6</v>
       </c>
       <c r="C9" s="47" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D9" s="48" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="48" t="s">
         <v>37</v>
-      </c>
-      <c r="E9" s="48" t="s">
-        <v>38</v>
       </c>
       <c r="F9" s="48"/>
       <c r="G9" s="57" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="60.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B10" s="18">
         <v>1</v>
       </c>
       <c r="C10" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="D10" s="28" t="s">
+      <c r="E10" s="28" t="s">
         <v>61</v>
-      </c>
-      <c r="E10" s="28" t="s">
-        <v>62</v>
       </c>
       <c r="F10" s="28"/>
       <c r="G10" s="27" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B11" s="18">
         <v>2</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D11" s="28" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E11" s="28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F11" s="28"/>
       <c r="G11" s="27" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B12" s="18">
         <v>3</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D12" s="28" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E12" s="28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F12" s="28"/>
       <c r="G12" s="27" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B13" s="18">
         <v>4</v>
       </c>
       <c r="C13" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="D13" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="E13" s="28" t="s">
+      <c r="F13" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="G13" s="27" t="s">
         <v>69</v>
-      </c>
-      <c r="F13" s="28" t="s">
-        <v>97</v>
-      </c>
-      <c r="G13" s="27" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B14" s="18">
         <v>5</v>
       </c>
       <c r="C14" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="D14" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" s="28" t="s">
         <v>71</v>
-      </c>
-      <c r="D14" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="E14" s="28" t="s">
-        <v>72</v>
       </c>
       <c r="F14" s="28"/>
       <c r="G14" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B15" s="18">
         <v>6</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D15" s="28" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E15" s="28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F15" s="28"/>
       <c r="G15" s="21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B16" s="18">
         <v>7</v>
       </c>
       <c r="C16" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="D16" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="28" t="s">
         <v>76</v>
-      </c>
-      <c r="D16" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="E16" s="28" t="s">
-        <v>77</v>
       </c>
       <c r="F16" s="28"/>
       <c r="G16" s="21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B17" s="18">
         <v>8</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D17" s="28" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E17" s="28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F17" s="28"/>
       <c r="G17" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="45" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B18" s="46">
         <v>9</v>
       </c>
       <c r="C18" s="47" t="s">
+        <v>80</v>
+      </c>
+      <c r="D18" s="48" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" s="48" t="s">
         <v>81</v>
-      </c>
-      <c r="D18" s="48" t="s">
-        <v>44</v>
-      </c>
-      <c r="E18" s="48" t="s">
-        <v>82</v>
       </c>
       <c r="F18" s="48"/>
       <c r="G18" s="49" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -7172,7 +7751,7 @@
       <c r="A20" s="24"/>
       <c r="B20" s="32"/>
       <c r="C20" s="34" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D20" s="25"/>
       <c r="E20" s="25"/>
@@ -7183,7 +7762,7 @@
       <c r="A21" s="24"/>
       <c r="B21" s="32"/>
       <c r="C21" s="35" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D21" s="25">
         <v>79</v>
@@ -7196,7 +7775,7 @@
       <c r="A22" s="24"/>
       <c r="B22" s="32"/>
       <c r="C22" s="35" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D22" s="25">
         <v>103</v>
@@ -7209,7 +7788,7 @@
       <c r="A23" s="36"/>
       <c r="B23" s="37"/>
       <c r="C23" s="38" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D23" s="39">
         <v>118</v>
@@ -7244,448 +7823,448 @@
       <c r="A1" s="8"/>
       <c r="B1" s="9"/>
       <c r="C1" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D1" s="43" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" s="13">
         <v>0</v>
       </c>
       <c r="C2" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="15" t="s">
         <v>27</v>
-      </c>
-      <c r="D2" s="15" t="s">
-        <v>28</v>
       </c>
       <c r="E2" s="15"/>
       <c r="F2" s="16"/>
     </row>
     <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" s="18">
         <v>0</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E3" s="20"/>
       <c r="F3" s="21"/>
     </row>
     <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4" s="18">
         <v>0</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E4" s="20"/>
       <c r="F4" s="21"/>
     </row>
     <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" s="18">
         <v>0</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E5" s="20"/>
       <c r="F5" s="21"/>
     </row>
     <row r="6" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B6" s="18">
         <v>1</v>
       </c>
       <c r="C6" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="E6" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="E6" s="23" t="s">
+      <c r="F6" s="21"/>
+    </row>
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="171" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="173">
+        <v>1</v>
+      </c>
+      <c r="C7" s="175" t="s">
         <v>35</v>
       </c>
-      <c r="F6" s="21"/>
-    </row>
-    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="165" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="167">
-        <v>1</v>
-      </c>
-      <c r="C7" s="169" t="s">
+      <c r="D7" s="177" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="171" t="s">
+      <c r="E7" s="179" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="173" t="s">
+      <c r="F7" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="F7" s="26" t="s">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="181"/>
+      <c r="B8" s="182"/>
+      <c r="C8" s="183"/>
+      <c r="D8" s="184"/>
+      <c r="E8" s="185"/>
+      <c r="F8" s="27" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="166"/>
-      <c r="B8" s="168"/>
-      <c r="C8" s="170"/>
-      <c r="D8" s="172"/>
-      <c r="E8" s="174"/>
-      <c r="F8" s="27" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" s="18">
         <v>2</v>
       </c>
       <c r="C9" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="D9" s="28" t="s">
+    </row>
+    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="171" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="173">
+        <v>3</v>
+      </c>
+      <c r="C10" s="175" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="177" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" s="177" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" s="26" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="181"/>
+      <c r="B11" s="182"/>
+      <c r="C11" s="183"/>
+      <c r="D11" s="184"/>
+      <c r="E11" s="184"/>
+      <c r="F11" s="21" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="171" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="173">
+        <v>4</v>
+      </c>
+      <c r="C12" s="175" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" s="177" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="177" t="s">
+        <v>48</v>
+      </c>
+      <c r="F12" s="26" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="181"/>
+      <c r="B13" s="182"/>
+      <c r="C13" s="183"/>
+      <c r="D13" s="184"/>
+      <c r="E13" s="184"/>
+      <c r="F13" s="21" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="171" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="173">
+        <v>5</v>
+      </c>
+      <c r="C14" s="175" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" s="177" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" s="177" t="s">
+        <v>52</v>
+      </c>
+      <c r="F14" s="26" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="181"/>
+      <c r="B15" s="182"/>
+      <c r="C15" s="183"/>
+      <c r="D15" s="184"/>
+      <c r="E15" s="184"/>
+      <c r="F15" s="27" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="171" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="173">
+        <v>6</v>
+      </c>
+      <c r="C16" s="175" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" s="177" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16" s="179" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="F9" s="21" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="165" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="167">
-        <v>3</v>
-      </c>
-      <c r="C10" s="169" t="s">
-        <v>43</v>
-      </c>
-      <c r="D10" s="171" t="s">
-        <v>44</v>
-      </c>
-      <c r="E10" s="171" t="s">
-        <v>45</v>
-      </c>
-      <c r="F10" s="26" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="166"/>
-      <c r="B11" s="168"/>
-      <c r="C11" s="170"/>
-      <c r="D11" s="172"/>
-      <c r="E11" s="172"/>
-      <c r="F11" s="21" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="165" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" s="167">
-        <v>4</v>
-      </c>
-      <c r="C12" s="169" t="s">
-        <v>48</v>
-      </c>
-      <c r="D12" s="171" t="s">
-        <v>37</v>
-      </c>
-      <c r="E12" s="171" t="s">
-        <v>49</v>
-      </c>
-      <c r="F12" s="26" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="166"/>
-      <c r="B13" s="168"/>
-      <c r="C13" s="170"/>
-      <c r="D13" s="172"/>
-      <c r="E13" s="172"/>
-      <c r="F13" s="21" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="165" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="167">
-        <v>5</v>
-      </c>
-      <c r="C14" s="169" t="s">
-        <v>52</v>
-      </c>
-      <c r="D14" s="171" t="s">
-        <v>37</v>
-      </c>
-      <c r="E14" s="171" t="s">
-        <v>53</v>
-      </c>
-      <c r="F14" s="26" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="166"/>
-      <c r="B15" s="168"/>
-      <c r="C15" s="170"/>
-      <c r="D15" s="172"/>
-      <c r="E15" s="172"/>
-      <c r="F15" s="27" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="165" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" s="167">
-        <v>6</v>
-      </c>
-      <c r="C16" s="169" t="s">
+      <c r="F16" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="D16" s="171" t="s">
-        <v>37</v>
-      </c>
-      <c r="E16" s="173" t="s">
-        <v>38</v>
-      </c>
-      <c r="F16" s="30" t="s">
+    </row>
+    <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="172"/>
+      <c r="B17" s="174"/>
+      <c r="C17" s="176"/>
+      <c r="D17" s="178"/>
+      <c r="E17" s="180"/>
+      <c r="F17" s="31" t="s">
         <v>57</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="175"/>
-      <c r="B17" s="176"/>
-      <c r="C17" s="177"/>
-      <c r="D17" s="178"/>
-      <c r="E17" s="179"/>
-      <c r="F17" s="31" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B18" s="18">
         <v>1</v>
       </c>
       <c r="C18" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="D18" s="28" t="s">
+      <c r="E18" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="E18" s="28" t="s">
+      <c r="F18" s="21" t="s">
         <v>62</v>
-      </c>
-      <c r="F18" s="21" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B19" s="18">
         <v>2</v>
       </c>
       <c r="C19" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="D19" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="F19" s="27" t="s">
         <v>64</v>
-      </c>
-      <c r="D19" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="E19" s="28" t="s">
-        <v>53</v>
-      </c>
-      <c r="F19" s="27" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B20" s="18">
         <v>3</v>
       </c>
       <c r="C20" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="D20" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="E20" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="F20" s="27" t="s">
         <v>66</v>
-      </c>
-      <c r="D20" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="E20" s="28" t="s">
-        <v>53</v>
-      </c>
-      <c r="F20" s="27" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B21" s="18">
         <v>4</v>
       </c>
       <c r="C21" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="E21" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="D21" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="E21" s="28" t="s">
+      <c r="F21" s="27" t="s">
         <v>69</v>
-      </c>
-      <c r="F21" s="27" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B22" s="18">
         <v>5</v>
       </c>
       <c r="C22" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="D22" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="D22" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="E22" s="28" t="s">
+      <c r="F22" s="21" t="s">
         <v>72</v>
-      </c>
-      <c r="F22" s="21" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B23" s="18">
         <v>6</v>
       </c>
       <c r="C23" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="D23" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="E23" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="F23" s="21" t="s">
         <v>74</v>
-      </c>
-      <c r="D23" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="E23" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="F23" s="21" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B24" s="18">
         <v>7</v>
       </c>
       <c r="C24" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="D24" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="E24" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="D24" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="E24" s="28" t="s">
+      <c r="F24" s="21" t="s">
         <v>77</v>
-      </c>
-      <c r="F24" s="21" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B25" s="18">
         <v>8</v>
       </c>
       <c r="C25" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="D25" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="E25" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="F25" s="21" t="s">
         <v>79</v>
-      </c>
-      <c r="D25" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="E25" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="F25" s="21" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B26" s="18">
         <v>9</v>
       </c>
       <c r="C26" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="D26" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="E26" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="D26" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="E26" s="28" t="s">
+      <c r="F26" s="21" t="s">
         <v>82</v>
-      </c>
-      <c r="F26" s="21" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -7700,7 +8279,7 @@
       <c r="A28" s="24"/>
       <c r="B28" s="32"/>
       <c r="C28" s="34" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D28" s="25"/>
       <c r="E28" s="25"/>
@@ -7710,7 +8289,7 @@
       <c r="A29" s="24"/>
       <c r="B29" s="32"/>
       <c r="C29" s="35" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D29" s="25">
         <v>79</v>
@@ -7722,7 +8301,7 @@
       <c r="A30" s="24"/>
       <c r="B30" s="32"/>
       <c r="C30" s="35" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D30" s="25">
         <v>103</v>
@@ -7734,7 +8313,7 @@
       <c r="A31" s="36"/>
       <c r="B31" s="37"/>
       <c r="C31" s="38" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D31" s="39">
         <v>118</v>
@@ -7743,31 +8322,31 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="C16:C17"/>
     <mergeCell ref="D16:D17"/>
     <mergeCell ref="E16:E17"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>